<commit_message>
Add Romania and corrected policy.
</commit_message>
<xml_diff>
--- a/data/p_urbanization.xlsx
+++ b/data/p_urbanization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\master_thesis\master_thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E15DFE-D95F-42D6-9818-71FA56DE1844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB7B940-88D4-4520-AE22-279DE8362C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="13300" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Development relevance</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Romania</t>
   </si>
 </sst>
 </file>
@@ -528,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1494,6 +1497,38 @@
       </c>
       <c r="J30">
         <v>53.908999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31">
+        <v>53.9</v>
+      </c>
+      <c r="C31">
+        <v>53.887</v>
+      </c>
+      <c r="D31">
+        <v>53.9</v>
+      </c>
+      <c r="E31">
+        <v>53.936</v>
+      </c>
+      <c r="F31">
+        <v>53.997999999999998</v>
+      </c>
+      <c r="G31">
+        <v>54.084000000000003</v>
+      </c>
+      <c r="H31">
+        <v>54.194000000000003</v>
+      </c>
+      <c r="I31">
+        <v>54.329000000000001</v>
+      </c>
+      <c r="J31">
+        <v>54.488999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>